<commit_message>
Added checkbox and foundation for collapse
</commit_message>
<xml_diff>
--- a/church_database/church_database.xlsx
+++ b/church_database/church_database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="481">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -31,21 +31,18 @@
     <t xml:space="preserve">Distance (mi)</t>
   </si>
   <si>
+    <t xml:space="preserve">Website Link</t>
+  </si>
+  <si>
     <t xml:space="preserve">Denomination</t>
   </si>
   <si>
-    <t xml:space="preserve">Website Link</t>
+    <t xml:space="preserve">Contact Email</t>
   </si>
   <si>
     <t xml:space="preserve">College Ministry?</t>
   </si>
   <si>
-    <t xml:space="preserve">Ministry Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact Email</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sunday worship times</t>
   </si>
   <si>
@@ -55,52 +52,127 @@
     <t xml:space="preserve">1110 Guadalupe St, Austin, TX 78701</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cccaustin.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">staff@cccaustin.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City Life Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">501 W 3rd St, Austin, TX 78701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://austincitylife.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">INFO@AUSTINCITYLIFE.ORG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University Christian Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007 University Ave, Austin, TX 78705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ucc-austin.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian Church, United Church of Christ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin@ucc-austin.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Presbyterian Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 E 8th St, Austin, TX 78701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cpcaustin.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presbyterian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cpcaustin.org/contact/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Saints' Episcopal Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">209 W 27th St, Austin, TX 78705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.allsaints-austin.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episcopal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connect@allsaints-austin.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First United Methodist Church of Austin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1201 Lavaca St, Austin, TX 78701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fumcaustin.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methodist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact@fumcaustin.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Austin Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1715 W Cesar Chavez St, Austin, TX 78703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://austinstone.org/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baptist</t>
   </si>
   <si>
-    <t xml:space="preserve">youtube.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jliew626@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Life Church</t>
-  </si>
-  <si>
-    <t xml:space="preserve">501 W 3rd St, Austin, TX 78701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University Christian Church</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2007 University Ave, Austin, TX 78705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Presbyterian Church</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200 E 8th St, Austin, TX 78701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All Saints' Episcopal Church</t>
-  </si>
-  <si>
-    <t xml:space="preserve">209 W 27th St, Austin, TX 78705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First United Methodist Church of Austin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1201 Lavaca St, Austin, TX 78701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Austin Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1715 W Cesar Chavez St, Austin, TX 78703</t>
+    <t xml:space="preserve">info@austinstone.org</t>
   </si>
   <si>
     <t xml:space="preserve">Church At East</t>
@@ -109,6 +181,9 @@
     <t xml:space="preserve">2830 Real St, Austin, TX 78722</t>
   </si>
   <si>
+    <t xml:space="preserve">http://www.churchateast.com/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gracepoint Austin Church</t>
   </si>
   <si>
@@ -895,268 +970,499 @@
     <t xml:space="preserve">Springdale Church of God in Christ</t>
   </si>
   <si>
+    <t xml:space="preserve">767 Springdale Rd, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saint Philip's Anglican Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1408 W 9th St, Austin, TX 78703</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grace First Community Church</t>
   </si>
   <si>
+    <t xml:space="preserve">6020 S 1st St, Austin, TX 78745</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Mark's Episcopal Church</t>
   </si>
   <si>
-    <t xml:space="preserve">Hyde Park Church</t>
+    <t xml:space="preserve">2128 Barton Hills Dr, Austin, TX 78704</t>
   </si>
   <si>
     <t xml:space="preserve">First Baptist Church Circle Drive</t>
   </si>
   <si>
+    <t xml:space="preserve">900 Neches St, Austin, TX 78701</t>
+  </si>
+  <si>
     <t xml:space="preserve">Victory Outreach Church</t>
   </si>
   <si>
     <t xml:space="preserve">Olivet Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1179 San Bernard St, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vision of Hope Church</t>
   </si>
   <si>
+    <t xml:space="preserve">Richardson Ln, Austin, TX 78741</t>
+  </si>
+  <si>
     <t xml:space="preserve">Holland Church of Christ</t>
   </si>
   <si>
+    <t xml:space="preserve">208 Adams St, Austin, TX 78729</t>
+  </si>
+  <si>
     <t xml:space="preserve">Central City Austin</t>
   </si>
   <si>
+    <t xml:space="preserve">9023 Old Lampasas Trail, Austin, TX 78750</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Jose Catholic Church</t>
   </si>
   <si>
+    <t xml:space="preserve">2435 Oak Crest Ave, Austin, TX 78704</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sacred Heart Catholic Church</t>
   </si>
   <si>
     <t xml:space="preserve">Christ Community Church</t>
   </si>
   <si>
+    <t xml:space="preserve">Christ Community Church, Austin, TX 78753</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bridge Church of Austin</t>
   </si>
   <si>
+    <t xml:space="preserve">950 Westbank Dr, West Lake Hills, TX 78746</t>
+  </si>
+  <si>
     <t xml:space="preserve">First Pentecostal Church of Austin</t>
   </si>
   <si>
+    <t xml:space="preserve">7440 Ed Bluestein Blvd, Austin, TX 78723</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Paul Primitive Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">St Paul Primitive Baptist Church, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Open Door Church of God in Christ</t>
   </si>
   <si>
+    <t xml:space="preserve">3317 E 12th St, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gateway Church South</t>
   </si>
   <si>
+    <t xml:space="preserve">6800 West Gate Blvd #120, Austin, TX 78745</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. John College Heights Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">7207 Carver Ave, Austin, TX 78752</t>
+  </si>
+  <si>
     <t xml:space="preserve">Teri Road Baptist Church</t>
   </si>
   <si>
-    <t xml:space="preserve">Sain Ignatius Martyr Catholic Church</t>
+    <t xml:space="preserve">1844 Teri Rd, Austin, TX 78744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint Ignatius Martyr Catholic Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126 W Oltorf St, Austin, TX 78704</t>
   </si>
   <si>
     <t xml:space="preserve">Faith Christian Center Church</t>
   </si>
   <si>
+    <t xml:space="preserve">6107 Manor Rd, Austin, TX 78723</t>
+  </si>
+  <si>
     <t xml:space="preserve">Woodlawn Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">4600 Menchaca Rd, Austin, TX 78745</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bethel Assembly of God</t>
   </si>
   <si>
+    <t xml:space="preserve">4322 Banister Ln, Austin, TX 78745</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cristo Rey Catholic Church</t>
   </si>
   <si>
+    <t xml:space="preserve">2208 E 2nd St, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Boulevard Church</t>
   </si>
   <si>
+    <t xml:space="preserve">Boulevard Church, Austin, TX 78744</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sweethome Missionary Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1725 W 11th St, Austin, TX 78703</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rosewood Avenue Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1820 Rosewood Ave, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Door of Hope Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1400 E Cesar Chavez St, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Our Lady of Guadalupe Parish</t>
   </si>
   <si>
+    <t xml:space="preserve">1206 E 9th St, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wildflower Church</t>
   </si>
   <si>
     <t xml:space="preserve">United Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1400 Guadalupe St, Austin, TX 78701</t>
+  </si>
+  <si>
     <t xml:space="preserve">East Side Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">2400 Northeast Dr, Austin, TX 78723</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seventh-Day Adventist Church</t>
   </si>
   <si>
     <t xml:space="preserve">Church of Pentecost</t>
   </si>
   <si>
+    <t xml:space="preserve">Church of Pentecost, 7801 N Lamar Blvd # D102, Austin, TX 78752</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greater Works Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">4000 Tannehill Ln, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ethiopian Evangelical Christian Church</t>
   </si>
   <si>
+    <t xml:space="preserve">305 Deen Ave, Austin, TX 78753</t>
+  </si>
+  <si>
     <t xml:space="preserve">Principe De Paz Christian Church</t>
   </si>
   <si>
     <t xml:space="preserve">Salem Lutheran Church</t>
   </si>
   <si>
+    <t xml:space="preserve">9322 FM812, Austin, TX 78719</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Apostolic Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1906 Miles Ave, Austin, TX 78745</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greater Peace Christian Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1203 E Cesar Chavez St, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Klegberg Hall</t>
   </si>
   <si>
+    <t xml:space="preserve">1201-1299 Ardenwood Rd, Austin, TX 78722</t>
+  </si>
+  <si>
     <t xml:space="preserve">Superior Church</t>
   </si>
   <si>
+    <t xml:space="preserve">900 Rio Grande St, Austin, TX 78701</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sta. Julia Church</t>
   </si>
   <si>
+    <t xml:space="preserve">3010 Lyons Rd, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Annie AME Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1711 Newton St, Austin, TX 78704</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greater Love Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">6601 Manor Rd, Austin, TX 78723</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mt. Olive Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1800 E 11th St #2718, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Antioch Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">4407 Monterey Oaks Blvd, Austin, TX 78749</t>
+  </si>
+  <si>
     <t xml:space="preserve">True Light Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">True Light Baptist Church, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">Agape Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">7801 N Lamar Blvd, Austin, TX 78752</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grant AME Worship Center</t>
   </si>
   <si>
+    <t xml:space="preserve">1701 Kramer Ln, Austin, TX 78758</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Hope Primitive Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1602 E M. Franklin Ave, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">Solid Rock Missionary Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1014 Gardner Rd, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Paul Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">501 Blackson Ave, Austin, TX 78752</t>
+  </si>
+  <si>
     <t xml:space="preserve">RCCG Cornerstone Church</t>
   </si>
   <si>
+    <t xml:space="preserve">7952 Anderson Square, Austin, TX 78757</t>
+  </si>
+  <si>
     <t xml:space="preserve">South Central Conference United Church of Christ</t>
   </si>
   <si>
+    <t xml:space="preserve">South Central Conference United Church of Christ, Austin, TX 78723</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rising Star Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1710 E 20th St, Austin, TX 78722</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Peter's United Methodist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">4509 Springdale Rd, Austin, TX 78723</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sanctuary Of Deliverance Church COGIC</t>
   </si>
   <si>
+    <t xml:space="preserve">1310 Salina St, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Foundation Christian Church</t>
   </si>
   <si>
+    <t xml:space="preserve">4402 S Congress Ave, Austin, TX 78745</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Lucas Lutheran Church</t>
   </si>
   <si>
+    <t xml:space="preserve">San Lucas Lutheran Church, Austin, TX 78704</t>
+  </si>
+  <si>
     <t xml:space="preserve">Austin Spirit of Life Deaf Church</t>
   </si>
   <si>
+    <t xml:space="preserve">7612 Cooper Ln, Austin, TX 78745</t>
+  </si>
+  <si>
     <t xml:space="preserve">Austin Good Korean Church of the Nazarene</t>
   </si>
   <si>
+    <t xml:space="preserve">9507 Dessau Rd, Austin, TX 78754</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fontaine Memorial Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1140 Ebert Ave # D, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">Praise Tabernacle Community Church</t>
   </si>
   <si>
+    <t xml:space="preserve">Praise Tabernacle Community Church, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emmanuel Bible Church of Christ</t>
   </si>
   <si>
+    <t xml:space="preserve">1144 Northwestern Ave, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Austin Central Hispana Seventh-Day Adventist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">415 Montopolis Dr, Austin, TX 78741</t>
+  </si>
+  <si>
     <t xml:space="preserve">University Catholic Center</t>
   </si>
   <si>
+    <t xml:space="preserve">2010 University Ave, Austin, TX 78705</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Luke Missionary Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1160 Hargrave St, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Good Shepherd Anglican Church</t>
   </si>
   <si>
+    <t xml:space="preserve">6700 Middle Fiskville Rd Suite #403, Austin, TX 78752</t>
+  </si>
+  <si>
     <t xml:space="preserve">International Restoration Church</t>
   </si>
   <si>
+    <t xml:space="preserve">10200 Sprinkle Rd, Austin, TX 78754</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greater Mount Moriah Primitive Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">4907 Springdale Rd, Austin, TX 78723</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Universal Church</t>
   </si>
   <si>
+    <t xml:space="preserve">9603 Dessau Rd, Austin, TX 78754</t>
+  </si>
+  <si>
     <t xml:space="preserve">Austin Central Seventh Day Adventist Church</t>
   </si>
   <si>
     <t xml:space="preserve">Austin Korean Presbyterian Church</t>
   </si>
   <si>
+    <t xml:space="preserve">12311 Natures Bend, Austin, TX 78753</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pilgrim Rest Primitive Baptist</t>
   </si>
   <si>
+    <t xml:space="preserve">3754 Bluestein Dr, Austin, TX 78721</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zion Hill Baptist Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1701 Chestnut Ave, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alpha Seventh-Day Adventist Church</t>
   </si>
   <si>
     <t xml:space="preserve">Capital City Church</t>
   </si>
   <si>
-    <t xml:space="preserve">Shepher of the Hills Lutheran</t>
+    <t xml:space="preserve">Shepherd of the Hills Lutheran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3525 Bee Cave Rd, Austin, TX 78746</t>
   </si>
   <si>
     <t xml:space="preserve">Vive Church</t>
   </si>
   <si>
+    <t xml:space="preserve">2105 San Antonio St, Austin, TX 78705</t>
+  </si>
+  <si>
     <t xml:space="preserve">St. Philips Missionary Baptist Church</t>
   </si>
   <si>
     <t xml:space="preserve">Austin District-United Methodist</t>
   </si>
   <si>
+    <t xml:space="preserve">1221 W Ben White Blvd # 201A, Austin, TX 78704</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hyde Park Chinese Baptist Church</t>
   </si>
   <si>
     <t xml:space="preserve">St. John's United Methodist</t>
   </si>
   <si>
+    <t xml:space="preserve">2140 Allandale Rd, Austin, TX 78756</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Testament Christian Church</t>
   </si>
   <si>
+    <t xml:space="preserve">1800 Pennsylvania Ave, Austin, TX 78702</t>
+  </si>
+  <si>
     <t xml:space="preserve">Life in the City</t>
   </si>
   <si>
+    <t xml:space="preserve">205 E Monroe St, Austin, TX 78704</t>
+  </si>
+  <si>
     <t xml:space="preserve">Celebration Church Central Austin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1006 W Koenig Ln, Austin, TX 78756</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1471,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="hh:mm\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -1191,13 +1497,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1245,8 +1551,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1254,15 +1568,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1285,13 +1595,13 @@
   </sheetPr>
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1316,9 +1626,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1334,32 +1642,30 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0.9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>0.416666666666667</v>
-      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -1377,19 +1683,27 @@
     </row>
     <row r="3" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1406,21 +1720,29 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1439,19 +1761,29 @@
     </row>
     <row r="5" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1470,21 +1802,35 @@
     </row>
     <row r="6" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1501,20 +1847,30 @@
     </row>
     <row r="7" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0.9</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1530,22 +1886,34 @@
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>2.8</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1563,15 +1931,17 @@
     </row>
     <row r="9" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>1.3</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1594,10 +1964,10 @@
     </row>
     <row r="10" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0.2</v>
@@ -1625,10 +1995,10 @@
     </row>
     <row r="11" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0.9</v>
@@ -1656,10 +2026,10 @@
     </row>
     <row r="12" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>2.1</v>
@@ -1687,10 +2057,10 @@
     </row>
     <row r="13" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1.5</v>
@@ -1718,10 +2088,10 @@
     </row>
     <row r="14" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0.8</v>
@@ -1749,10 +2119,10 @@
     </row>
     <row r="15" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>1.1</v>
@@ -1780,10 +2150,10 @@
     </row>
     <row r="16" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.5</v>
@@ -1811,10 +2181,10 @@
     </row>
     <row r="17" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>1.1</v>
@@ -1842,10 +2212,10 @@
     </row>
     <row r="18" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0.2</v>
@@ -1873,10 +2243,10 @@
     </row>
     <row r="19" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0.9</v>
@@ -1902,12 +2272,12 @@
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.1</v>
@@ -1935,10 +2305,10 @@
     </row>
     <row r="21" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1.1</v>
@@ -1966,10 +2336,10 @@
     </row>
     <row r="22" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>6.9</v>
@@ -1995,12 +2365,12 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>7.9</v>
@@ -2028,10 +2398,10 @@
     </row>
     <row r="24" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>4.4</v>
@@ -2057,12 +2427,12 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>3.1</v>
@@ -2090,10 +2460,10 @@
     </row>
     <row r="26" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>5.7</v>
@@ -2121,10 +2491,10 @@
     </row>
     <row r="27" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>3.3</v>
@@ -2152,10 +2522,10 @@
     </row>
     <row r="28" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>8.9</v>
@@ -2183,10 +2553,10 @@
     </row>
     <row r="29" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>9.4</v>
@@ -2214,10 +2584,10 @@
     </row>
     <row r="30" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>6.4</v>
@@ -2243,12 +2613,12 @@
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>4.1</v>
@@ -2276,10 +2646,10 @@
     </row>
     <row r="32" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>4</v>
@@ -2307,10 +2677,10 @@
     </row>
     <row r="33" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>3.7</v>
@@ -2338,10 +2708,10 @@
     </row>
     <row r="34" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>3.7</v>
@@ -2369,10 +2739,10 @@
     </row>
     <row r="35" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>7.3</v>
@@ -2398,12 +2768,12 @@
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>10</v>
@@ -2431,10 +2801,10 @@
     </row>
     <row r="37" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>10.2</v>
@@ -2462,10 +2832,10 @@
     </row>
     <row r="38" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>3.1</v>
@@ -2493,10 +2863,10 @@
     </row>
     <row r="39" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0.2</v>
@@ -2524,10 +2894,10 @@
     </row>
     <row r="40" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>10.8</v>
@@ -2555,10 +2925,10 @@
     </row>
     <row r="41" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>1.3</v>
@@ -2586,10 +2956,10 @@
     </row>
     <row r="42" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>1.5</v>
@@ -2615,12 +2985,12 @@
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>1.2</v>
@@ -2648,10 +3018,10 @@
     </row>
     <row r="44" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>10.4</v>
@@ -2679,10 +3049,10 @@
     </row>
     <row r="45" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>3.5</v>
@@ -2708,12 +3078,12 @@
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>10.4</v>
@@ -2741,10 +3111,10 @@
     </row>
     <row r="47" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>7.8</v>
@@ -2770,12 +3140,12 @@
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>0.5</v>
@@ -2803,10 +3173,10 @@
     </row>
     <row r="49" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>0.4</v>
@@ -2834,10 +3204,10 @@
     </row>
     <row r="50" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>7.1</v>
@@ -2865,10 +3235,10 @@
     </row>
     <row r="51" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>4.4</v>
@@ -2894,12 +3264,12 @@
       <c r="V51" s="2"/>
       <c r="W51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>4</v>
@@ -2925,12 +3295,12 @@
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>3.6</v>
@@ -2958,10 +3328,10 @@
     </row>
     <row r="54" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>0.1</v>
@@ -2987,12 +3357,12 @@
       <c r="V54" s="2"/>
       <c r="W54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>4.3</v>
@@ -3020,10 +3390,10 @@
     </row>
     <row r="56" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>2.5</v>
@@ -3051,10 +3421,10 @@
     </row>
     <row r="57" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>2.6</v>
@@ -3082,10 +3452,10 @@
     </row>
     <row r="58" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>9.1</v>
@@ -3113,10 +3483,10 @@
     </row>
     <row r="59" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>3.2</v>
@@ -3142,12 +3512,12 @@
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0.4</v>
@@ -3175,10 +3545,10 @@
     </row>
     <row r="61" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>7.5</v>
@@ -3206,10 +3576,10 @@
     </row>
     <row r="62" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>1.5</v>
@@ -3237,10 +3607,10 @@
     </row>
     <row r="63" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>1.3</v>
@@ -3268,10 +3638,10 @@
     </row>
     <row r="64" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>7.2</v>
@@ -3299,10 +3669,10 @@
     </row>
     <row r="65" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>8.6</v>
@@ -3330,10 +3700,10 @@
     </row>
     <row r="66" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>2.2</v>
@@ -3361,10 +3731,10 @@
     </row>
     <row r="67" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>3.3</v>
@@ -3392,10 +3762,10 @@
     </row>
     <row r="68" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>3.9</v>
@@ -3423,10 +3793,10 @@
     </row>
     <row r="69" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>0.6</v>
@@ -3452,12 +3822,12 @@
       <c r="V69" s="2"/>
       <c r="W69" s="2"/>
     </row>
-    <row r="70" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>1.3</v>
@@ -3485,10 +3855,10 @@
     </row>
     <row r="71" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>4.2</v>
@@ -3516,10 +3886,10 @@
     </row>
     <row r="72" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>8.8</v>
@@ -3545,12 +3915,12 @@
       <c r="V72" s="2"/>
       <c r="W72" s="2"/>
     </row>
-    <row r="73" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>10</v>
@@ -3576,12 +3946,12 @@
       <c r="V73" s="2"/>
       <c r="W73" s="2"/>
     </row>
-    <row r="74" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>5</v>
@@ -3609,10 +3979,10 @@
     </row>
     <row r="75" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>4.6</v>
@@ -3640,10 +4010,10 @@
     </row>
     <row r="76" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>7</v>
@@ -3671,10 +4041,10 @@
     </row>
     <row r="77" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>5</v>
@@ -3700,12 +4070,12 @@
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
     </row>
-    <row r="78" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>3</v>
@@ -3733,10 +4103,10 @@
     </row>
     <row r="79" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>10.7</v>
@@ -3762,12 +4132,12 @@
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
     </row>
-    <row r="80" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>2.8</v>
@@ -3793,12 +4163,12 @@
       <c r="V80" s="2"/>
       <c r="W80" s="2"/>
     </row>
-    <row r="81" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>5</v>
@@ -3826,10 +4196,10 @@
     </row>
     <row r="82" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>5</v>
@@ -3857,10 +4227,10 @@
     </row>
     <row r="83" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>2.4</v>
@@ -3888,10 +4258,10 @@
     </row>
     <row r="84" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>3.1</v>
@@ -3917,12 +4287,12 @@
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
     </row>
-    <row r="85" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>2.7</v>
@@ -3948,12 +4318,12 @@
       <c r="V85" s="2"/>
       <c r="W85" s="2"/>
     </row>
-    <row r="86" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>1.8</v>
@@ -3981,10 +4351,10 @@
     </row>
     <row r="87" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>1.2</v>
@@ -4012,10 +4382,10 @@
     </row>
     <row r="88" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>1.9</v>
@@ -4041,12 +4411,12 @@
       <c r="V88" s="2"/>
       <c r="W88" s="2"/>
     </row>
-    <row r="89" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>3.4</v>
@@ -4074,10 +4444,10 @@
     </row>
     <row r="90" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>8.4</v>
@@ -4105,10 +4475,10 @@
     </row>
     <row r="91" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>4</v>
@@ -4136,10 +4506,10 @@
     </row>
     <row r="92" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>3.8</v>
@@ -4167,10 +4537,10 @@
     </row>
     <row r="93" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>0.6</v>
@@ -4198,10 +4568,10 @@
     </row>
     <row r="94" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>2.7</v>
@@ -4227,12 +4597,12 @@
       <c r="V94" s="2"/>
       <c r="W94" s="2"/>
     </row>
-    <row r="95" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>10</v>
@@ -4258,12 +4628,12 @@
       <c r="V95" s="2"/>
       <c r="W95" s="2"/>
     </row>
-    <row r="96" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>10</v>
@@ -4291,10 +4661,10 @@
     </row>
     <row r="97" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>7</v>
@@ -4322,10 +4692,10 @@
     </row>
     <row r="98" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="C98" s="1" t="n">
         <v>10.2</v>
@@ -4351,12 +4721,12 @@
       <c r="V98" s="2"/>
       <c r="W98" s="2"/>
     </row>
-    <row r="99" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="C99" s="1" t="n">
         <v>1.4</v>
@@ -4382,12 +4752,12 @@
       <c r="V99" s="2"/>
       <c r="W99" s="2"/>
     </row>
-    <row r="100" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>2.7</v>
@@ -4415,10 +4785,10 @@
     </row>
     <row r="101" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>6.1</v>
@@ -4446,10 +4816,10 @@
     </row>
     <row r="102" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>1.9</v>
@@ -4477,10 +4847,10 @@
     </row>
     <row r="103" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>3.5</v>
@@ -4508,10 +4878,10 @@
     </row>
     <row r="104" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>4.2</v>
@@ -4539,10 +4909,10 @@
     </row>
     <row r="105" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>4.2</v>
@@ -4570,10 +4940,10 @@
     </row>
     <row r="106" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>3.8</v>
@@ -4601,10 +4971,10 @@
     </row>
     <row r="107" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>214</v>
+        <v>239</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="C107" s="1" t="n">
         <v>5.7</v>
@@ -4630,12 +5000,12 @@
       <c r="V107" s="2"/>
       <c r="W107" s="2"/>
     </row>
-    <row r="108" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>4.4</v>
@@ -4663,10 +5033,10 @@
     </row>
     <row r="109" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>3.5</v>
@@ -4692,12 +5062,12 @@
       <c r="V109" s="2"/>
       <c r="W109" s="2"/>
     </row>
-    <row r="110" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="C110" s="1" t="n">
         <v>11.2</v>
@@ -4725,10 +5095,10 @@
     </row>
     <row r="111" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C111" s="1" t="n">
         <v>0.9</v>
@@ -4756,10 +5126,10 @@
     </row>
     <row r="112" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>223</v>
+        <v>248</v>
       </c>
       <c r="C112" s="1" t="n">
         <v>2.2</v>
@@ -4787,10 +5157,10 @@
     </row>
     <row r="113" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>6.1</v>
@@ -4818,10 +5188,10 @@
     </row>
     <row r="114" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
       <c r="C114" s="1" t="n">
         <v>8.6</v>
@@ -4849,10 +5219,10 @@
     </row>
     <row r="115" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="C115" s="1" t="n">
         <v>0.8</v>
@@ -4878,12 +5248,12 @@
       <c r="V115" s="2"/>
       <c r="W115" s="2"/>
     </row>
-    <row r="116" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="C116" s="1" t="n">
         <v>0.9</v>
@@ -4909,12 +5279,12 @@
       <c r="V116" s="2"/>
       <c r="W116" s="2"/>
     </row>
-    <row r="117" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>2.8</v>
@@ -4942,10 +5312,10 @@
     </row>
     <row r="118" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>4.1</v>
@@ -4973,10 +5343,10 @@
     </row>
     <row r="119" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>1</v>
@@ -5002,12 +5372,12 @@
       <c r="V119" s="2"/>
       <c r="W119" s="2"/>
     </row>
-    <row r="120" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="C120" s="1" t="n">
         <v>2</v>
@@ -5035,10 +5405,10 @@
     </row>
     <row r="121" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>1.3</v>
@@ -5066,10 +5436,10 @@
     </row>
     <row r="122" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="C122" s="1" t="n">
         <v>2.9</v>
@@ -5097,10 +5467,10 @@
     </row>
     <row r="123" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="C123" s="1" t="n">
         <v>3.8</v>
@@ -5126,12 +5496,12 @@
       <c r="V123" s="2"/>
       <c r="W123" s="2"/>
     </row>
-    <row r="124" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="C124" s="1" t="n">
         <v>3.9</v>
@@ -5157,12 +5527,12 @@
       <c r="V124" s="2"/>
       <c r="W124" s="2"/>
     </row>
-    <row r="125" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>1.1</v>
@@ -5190,10 +5560,10 @@
     </row>
     <row r="126" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>2.7</v>
@@ -5219,12 +5589,12 @@
       <c r="V126" s="2"/>
       <c r="W126" s="2"/>
     </row>
-    <row r="127" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>8.5</v>
@@ -5252,10 +5622,10 @@
     </row>
     <row r="128" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="C128" s="1" t="n">
         <v>4.5</v>
@@ -5281,12 +5651,12 @@
       <c r="V128" s="2"/>
       <c r="W128" s="2"/>
     </row>
-    <row r="129" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="C129" s="1" t="n">
         <v>7.2</v>
@@ -5314,10 +5684,10 @@
     </row>
     <row r="130" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="C130" s="1" t="n">
         <v>0.8</v>
@@ -5345,10 +5715,10 @@
     </row>
     <row r="131" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>261</v>
+        <v>286</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>1</v>
@@ -5376,10 +5746,10 @@
     </row>
     <row r="132" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>262</v>
+        <v>287</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="C132" s="1" t="n">
         <v>2.7</v>
@@ -5407,10 +5777,10 @@
     </row>
     <row r="133" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>264</v>
+        <v>289</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="C133" s="1" t="n">
         <v>3.5</v>
@@ -5438,10 +5808,10 @@
     </row>
     <row r="134" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="C134" s="1" t="n">
         <v>3.2</v>
@@ -5469,10 +5839,10 @@
     </row>
     <row r="135" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>269</v>
+        <v>294</v>
       </c>
       <c r="C135" s="1" t="n">
         <v>3.5</v>
@@ -5500,10 +5870,10 @@
     </row>
     <row r="136" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C136" s="1" t="n">
         <v>7.2</v>
@@ -5531,10 +5901,10 @@
     </row>
     <row r="137" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>271</v>
+        <v>296</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="C137" s="1" t="n">
         <v>0.1</v>
@@ -5562,10 +5932,10 @@
     </row>
     <row r="138" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>5.7</v>
@@ -5591,12 +5961,12 @@
       <c r="V138" s="2"/>
       <c r="W138" s="2"/>
     </row>
-    <row r="139" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>3.8</v>
@@ -5624,10 +5994,10 @@
     </row>
     <row r="140" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>277</v>
+        <v>302</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>0.3</v>
@@ -5655,10 +6025,10 @@
     </row>
     <row r="141" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>5.5</v>
@@ -5684,12 +6054,12 @@
       <c r="V141" s="2"/>
       <c r="W141" s="2"/>
     </row>
-    <row r="142" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>3.5</v>
@@ -5715,12 +6085,12 @@
       <c r="V142" s="2"/>
       <c r="W142" s="2"/>
     </row>
-    <row r="143" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>6.2</v>
@@ -5748,10 +6118,10 @@
     </row>
     <row r="144" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="C144" s="1" t="n">
         <v>1.3</v>
@@ -5779,10 +6149,10 @@
     </row>
     <row r="145" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>287</v>
+        <v>312</v>
       </c>
       <c r="C145" s="1" t="n">
         <v>2.8</v>
@@ -5810,10 +6180,10 @@
     </row>
     <row r="146" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>288</v>
+        <v>313</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="C146" s="1" t="n">
         <v>10.2</v>
@@ -5839,12 +6209,16 @@
       <c r="V146" s="2"/>
       <c r="W146" s="2"/>
     </row>
-    <row r="147" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
+        <v>315</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C147" s="1" t="n">
+        <v>3.4</v>
+      </c>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
@@ -5868,10 +6242,14 @@
     </row>
     <row r="148" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
+        <v>317</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C148" s="1" t="n">
+        <v>2.2</v>
+      </c>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
@@ -5895,10 +6273,14 @@
     </row>
     <row r="149" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
+        <v>319</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C149" s="1" t="n">
+        <v>6.8</v>
+      </c>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
@@ -5920,12 +6302,16 @@
       <c r="V149" s="2"/>
       <c r="W149" s="2"/>
     </row>
-    <row r="150" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C150" s="1" t="n">
+        <v>4.9</v>
+      </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
@@ -5947,12 +6333,16 @@
       <c r="V150" s="2"/>
       <c r="W150" s="2"/>
     </row>
-    <row r="151" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
+        <v>323</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C151" s="1" t="n">
+        <v>1.2</v>
+      </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
@@ -5976,10 +6366,14 @@
     </row>
     <row r="152" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
+        <v>325</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C152" s="1" t="n">
+        <v>10.5</v>
+      </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
       <c r="F152" s="2"/>
@@ -6001,12 +6395,16 @@
       <c r="V152" s="2"/>
       <c r="W152" s="2"/>
     </row>
-    <row r="153" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
+        <v>326</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C153" s="1" t="n">
+        <v>1.4</v>
+      </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
@@ -6028,12 +6426,16 @@
       <c r="V153" s="2"/>
       <c r="W153" s="2"/>
     </row>
-    <row r="154" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
+        <v>328</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C154" s="1" t="n">
+        <v>5.2</v>
+      </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="F154" s="2"/>
@@ -6055,12 +6457,16 @@
       <c r="V154" s="2"/>
       <c r="W154" s="2"/>
     </row>
-    <row r="155" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C155" s="1" t="n">
+        <v>2.5</v>
+      </c>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
@@ -6082,12 +6488,16 @@
       <c r="V155" s="2"/>
       <c r="W155" s="2"/>
     </row>
-    <row r="156" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
+        <v>332</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C156" s="1" t="n">
+        <v>12.6</v>
+      </c>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
@@ -6109,12 +6519,16 @@
       <c r="V156" s="2"/>
       <c r="W156" s="2"/>
     </row>
-    <row r="157" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C157" s="1" t="n">
+        <v>3.9</v>
+      </c>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
@@ -6136,12 +6550,16 @@
       <c r="V157" s="2"/>
       <c r="W157" s="2"/>
     </row>
-    <row r="158" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
+        <v>336</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C158" s="1" t="n">
+        <v>4.4</v>
+      </c>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -6163,12 +6581,16 @@
       <c r="V158" s="2"/>
       <c r="W158" s="2"/>
     </row>
-    <row r="159" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
+        <v>337</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C159" s="1" t="n">
+        <v>7.9</v>
+      </c>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
@@ -6190,12 +6612,16 @@
       <c r="V159" s="2"/>
       <c r="W159" s="2"/>
     </row>
-    <row r="160" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
+        <v>339</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C160" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
@@ -6217,12 +6643,16 @@
       <c r="V160" s="2"/>
       <c r="W160" s="2"/>
     </row>
-    <row r="161" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
+        <v>341</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C161" s="1" t="n">
+        <v>5.5</v>
+      </c>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
@@ -6244,12 +6674,16 @@
       <c r="V161" s="2"/>
       <c r="W161" s="2"/>
     </row>
-    <row r="162" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="68.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C162" s="1" t="n">
+        <v>1.6</v>
+      </c>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
@@ -6273,10 +6707,14 @@
     </row>
     <row r="163" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
+        <v>345</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C163" s="1" t="n">
+        <v>2.5</v>
+      </c>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
@@ -6298,12 +6736,16 @@
       <c r="V163" s="2"/>
       <c r="W163" s="2"/>
     </row>
-    <row r="164" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
+        <v>347</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C164" s="1" t="n">
+        <v>8.2</v>
+      </c>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
@@ -6325,12 +6767,16 @@
       <c r="V164" s="2"/>
       <c r="W164" s="2"/>
     </row>
-    <row r="165" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
+        <v>349</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C165" s="1" t="n">
+        <v>4.3</v>
+      </c>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
@@ -6352,12 +6798,16 @@
       <c r="V165" s="2"/>
       <c r="W165" s="2"/>
     </row>
-    <row r="166" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
+        <v>351</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C166" s="1" t="n">
+        <v>6.5</v>
+      </c>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
@@ -6379,12 +6829,16 @@
       <c r="V166" s="2"/>
       <c r="W166" s="2"/>
     </row>
-    <row r="167" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C167" s="1" t="n">
+        <v>3.7</v>
+      </c>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
@@ -6408,10 +6862,14 @@
     </row>
     <row r="168" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
+        <v>355</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C168" s="1" t="n">
+        <v>4.3</v>
+      </c>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
@@ -6433,12 +6891,16 @@
       <c r="V168" s="2"/>
       <c r="W168" s="2"/>
     </row>
-    <row r="169" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
+        <v>357</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C169" s="1" t="n">
+        <v>6.1</v>
+      </c>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
@@ -6460,12 +6922,16 @@
       <c r="V169" s="2"/>
       <c r="W169" s="2"/>
     </row>
-    <row r="170" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
+        <v>359</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C170" s="1" t="n">
+        <v>5.7</v>
+      </c>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
@@ -6489,10 +6955,14 @@
     </row>
     <row r="171" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
+        <v>361</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C171" s="1" t="n">
+        <v>2.7</v>
+      </c>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
@@ -6514,12 +6984,16 @@
       <c r="V171" s="2"/>
       <c r="W171" s="2"/>
     </row>
-    <row r="172" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
+        <v>363</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C172" s="1" t="n">
+        <v>6.9</v>
+      </c>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
@@ -6541,12 +7015,16 @@
       <c r="V172" s="2"/>
       <c r="W172" s="2"/>
     </row>
-    <row r="173" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
+        <v>365</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C173" s="1" t="n">
+        <v>2.3</v>
+      </c>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
@@ -6568,12 +7046,16 @@
       <c r="V173" s="2"/>
       <c r="W173" s="2"/>
     </row>
-    <row r="174" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
+        <v>367</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C174" s="1" t="n">
+        <v>1.7</v>
+      </c>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
@@ -6595,12 +7077,16 @@
       <c r="V174" s="2"/>
       <c r="W174" s="2"/>
     </row>
-    <row r="175" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C175" s="1" t="n">
+        <v>2.3</v>
+      </c>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
@@ -6622,12 +7108,16 @@
       <c r="V175" s="2"/>
       <c r="W175" s="2"/>
     </row>
-    <row r="176" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C176" s="1" t="n">
+        <v>1.7</v>
+      </c>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
@@ -6651,10 +7141,14 @@
     </row>
     <row r="177" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
+        <v>373</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C177" s="1" t="n">
+        <v>4.2</v>
+      </c>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
@@ -6676,12 +7170,16 @@
       <c r="V177" s="2"/>
       <c r="W177" s="2"/>
     </row>
-    <row r="178" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
+        <v>374</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C178" s="1" t="n">
+        <v>1.1</v>
+      </c>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
@@ -6703,12 +7201,16 @@
       <c r="V178" s="2"/>
       <c r="W178" s="2"/>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
+        <v>376</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C179" s="1" t="n">
+        <v>4.7</v>
+      </c>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
@@ -6730,12 +7232,16 @@
       <c r="V179" s="2"/>
       <c r="W179" s="2"/>
     </row>
-    <row r="180" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
+        <v>378</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C180" s="1" t="n">
+        <v>0.9</v>
+      </c>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
@@ -6757,12 +7263,16 @@
       <c r="V180" s="2"/>
       <c r="W180" s="2"/>
     </row>
-    <row r="181" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="68.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
+        <v>379</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C181" s="1" t="n">
+        <v>4.9</v>
+      </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
@@ -6784,12 +7294,16 @@
       <c r="V181" s="2"/>
       <c r="W181" s="2"/>
     </row>
-    <row r="182" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
+        <v>381</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C182" s="1" t="n">
+        <v>4.1</v>
+      </c>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
@@ -6811,12 +7325,16 @@
       <c r="V182" s="2"/>
       <c r="W182" s="2"/>
     </row>
-    <row r="183" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
+        <v>383</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C183" s="1" t="n">
+        <v>5.7</v>
+      </c>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
@@ -6840,10 +7358,14 @@
     </row>
     <row r="184" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
+        <v>385</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C184" s="1" t="n">
+        <v>3.9</v>
+      </c>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
@@ -6867,10 +7389,14 @@
     </row>
     <row r="185" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
+        <v>386</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C185" s="1" t="n">
+        <v>11.1</v>
+      </c>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
@@ -6894,10 +7420,14 @@
     </row>
     <row r="186" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
+        <v>388</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C186" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
@@ -6919,12 +7449,16 @@
       <c r="V186" s="2"/>
       <c r="W186" s="2"/>
     </row>
-    <row r="187" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
+        <v>390</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C187" s="1" t="n">
+        <v>2.1</v>
+      </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
@@ -6946,12 +7480,16 @@
       <c r="V187" s="2"/>
       <c r="W187" s="2"/>
     </row>
-    <row r="188" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
+        <v>392</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C188" s="1" t="n">
+        <v>1.8</v>
+      </c>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
@@ -6973,12 +7511,16 @@
       <c r="V188" s="2"/>
       <c r="W188" s="2"/>
     </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
+        <v>394</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C189" s="1" t="n">
+        <v>1.3</v>
+      </c>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
@@ -7000,12 +7542,16 @@
       <c r="V189" s="2"/>
       <c r="W189" s="2"/>
     </row>
-    <row r="190" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
+        <v>396</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C190" s="1" t="n">
+        <v>2.4</v>
+      </c>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
@@ -7027,12 +7573,16 @@
       <c r="V190" s="2"/>
       <c r="W190" s="2"/>
     </row>
-    <row r="191" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
+        <v>398</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C191" s="1" t="n">
+        <v>2.9</v>
+      </c>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
@@ -7054,12 +7604,16 @@
       <c r="V191" s="2"/>
       <c r="W191" s="2"/>
     </row>
-    <row r="192" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
+        <v>400</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C192" s="1" t="n">
+        <v>4.4</v>
+      </c>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
@@ -7081,12 +7635,16 @@
       <c r="V192" s="2"/>
       <c r="W192" s="2"/>
     </row>
-    <row r="193" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C193" s="1" t="n">
+        <v>1.4</v>
+      </c>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
@@ -7108,12 +7666,16 @@
       <c r="V193" s="2"/>
       <c r="W193" s="2"/>
     </row>
-    <row r="194" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B194" s="2"/>
-      <c r="C194" s="2"/>
+        <v>404</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C194" s="1" t="n">
+        <v>8.2</v>
+      </c>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
@@ -7135,12 +7697,16 @@
       <c r="V194" s="2"/>
       <c r="W194" s="2"/>
     </row>
-    <row r="195" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B195" s="2"/>
-      <c r="C195" s="2"/>
+        <v>406</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C195" s="1" t="n">
+        <v>3.5</v>
+      </c>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
       <c r="F195" s="2"/>
@@ -7162,12 +7728,16 @@
       <c r="V195" s="2"/>
       <c r="W195" s="2"/>
     </row>
-    <row r="196" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B196" s="2"/>
-      <c r="C196" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C196" s="1" t="n">
+        <v>4.5</v>
+      </c>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
       <c r="F196" s="2"/>
@@ -7189,12 +7759,16 @@
       <c r="V196" s="2"/>
       <c r="W196" s="2"/>
     </row>
-    <row r="197" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="B197" s="2"/>
-      <c r="C197" s="2"/>
+        <v>410</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C197" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
@@ -7216,12 +7790,16 @@
       <c r="V197" s="2"/>
       <c r="W197" s="2"/>
     </row>
-    <row r="198" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
+        <v>412</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C198" s="1" t="n">
+        <v>2.3</v>
+      </c>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
@@ -7243,12 +7821,16 @@
       <c r="V198" s="2"/>
       <c r="W198" s="2"/>
     </row>
-    <row r="199" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B199" s="2"/>
-      <c r="C199" s="2"/>
+        <v>414</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C199" s="1" t="n">
+        <v>3.8</v>
+      </c>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
@@ -7272,10 +7854,14 @@
     </row>
     <row r="200" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B200" s="2"/>
-      <c r="C200" s="2"/>
+        <v>416</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C200" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
@@ -7297,12 +7883,16 @@
       <c r="V200" s="2"/>
       <c r="W200" s="2"/>
     </row>
-    <row r="201" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B201" s="2"/>
-      <c r="C201" s="2"/>
+        <v>418</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C201" s="1" t="n">
+        <v>4.9</v>
+      </c>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
@@ -7324,12 +7914,16 @@
       <c r="V201" s="2"/>
       <c r="W201" s="2"/>
     </row>
-    <row r="202" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="79.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B202" s="2"/>
-      <c r="C202" s="2"/>
+        <v>420</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C202" s="1" t="n">
+        <v>3.3</v>
+      </c>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
@@ -7351,12 +7945,16 @@
       <c r="V202" s="2"/>
       <c r="W202" s="2"/>
     </row>
-    <row r="203" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="B203" s="2"/>
-      <c r="C203" s="2"/>
+        <v>422</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C203" s="1" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
       <c r="F203" s="2"/>
@@ -7378,12 +7976,16 @@
       <c r="V203" s="2"/>
       <c r="W203" s="2"/>
     </row>
-    <row r="204" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B204" s="2"/>
-      <c r="C204" s="2"/>
+        <v>424</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C204" s="1" t="n">
+        <v>3.1</v>
+      </c>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
       <c r="F204" s="2"/>
@@ -7407,10 +8009,14 @@
     </row>
     <row r="205" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B205" s="2"/>
-      <c r="C205" s="2"/>
+        <v>426</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C205" s="1" t="n">
+        <v>0.9</v>
+      </c>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
@@ -7434,10 +8040,14 @@
     </row>
     <row r="206" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B206" s="2"/>
-      <c r="C206" s="2"/>
+        <v>428</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C206" s="1" t="n">
+        <v>5.1</v>
+      </c>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
@@ -7459,12 +8069,16 @@
       <c r="V206" s="2"/>
       <c r="W206" s="2"/>
     </row>
-    <row r="207" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B207" s="2"/>
-      <c r="C207" s="2"/>
+        <v>430</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C207" s="1" t="n">
+        <v>4.7</v>
+      </c>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
@@ -7488,10 +8102,14 @@
     </row>
     <row r="208" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B208" s="2"/>
-      <c r="C208" s="2"/>
+        <v>432</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C208" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
@@ -7513,12 +8131,16 @@
       <c r="V208" s="2"/>
       <c r="W208" s="2"/>
     </row>
-    <row r="209" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="B209" s="2"/>
-      <c r="C209" s="2"/>
+        <v>434</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C209" s="1" t="n">
+        <v>5.8</v>
+      </c>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
       <c r="F209" s="2"/>
@@ -7542,10 +8164,14 @@
     </row>
     <row r="210" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B210" s="2"/>
-      <c r="C210" s="2"/>
+        <v>436</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C210" s="1" t="n">
+        <v>3.2</v>
+      </c>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
       <c r="F210" s="2"/>
@@ -7567,12 +8193,16 @@
       <c r="V210" s="2"/>
       <c r="W210" s="2"/>
     </row>
-    <row r="211" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="68.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B211" s="2"/>
-      <c r="C211" s="2"/>
+        <v>438</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C211" s="1" t="n">
+        <v>4.2</v>
+      </c>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
       <c r="F211" s="2"/>
@@ -7596,10 +8226,14 @@
     </row>
     <row r="212" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B212" s="2"/>
-      <c r="C212" s="2"/>
+        <v>440</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C212" s="1" t="n">
+        <v>1.5</v>
+      </c>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
       <c r="F212" s="2"/>
@@ -7621,12 +8255,16 @@
       <c r="V212" s="2"/>
       <c r="W212" s="2"/>
     </row>
-    <row r="213" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="68.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="B213" s="2"/>
-      <c r="C213" s="2"/>
+        <v>442</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C213" s="1" t="n">
+        <v>4.4</v>
+      </c>
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="2"/>
@@ -7648,12 +8286,16 @@
       <c r="V213" s="2"/>
       <c r="W213" s="2"/>
     </row>
-    <row r="214" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
+        <v>444</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C214" s="1" t="n">
+        <v>0.4</v>
+      </c>
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
@@ -7675,12 +8317,16 @@
       <c r="V214" s="2"/>
       <c r="W214" s="2"/>
     </row>
-    <row r="215" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
+        <v>446</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C215" s="1" t="n">
+        <v>1.9</v>
+      </c>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
@@ -7702,12 +8348,16 @@
       <c r="V215" s="2"/>
       <c r="W215" s="2"/>
     </row>
-    <row r="216" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
+        <v>448</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C216" s="1" t="n">
+        <v>3.3</v>
+      </c>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
@@ -7731,10 +8381,14 @@
     </row>
     <row r="217" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
+        <v>450</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C217" s="1" t="n">
+        <v>7.3</v>
+      </c>
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
@@ -7756,12 +8410,16 @@
       <c r="V217" s="2"/>
       <c r="W217" s="2"/>
     </row>
-    <row r="218" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="B218" s="2"/>
-      <c r="C218" s="2"/>
+        <v>452</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C218" s="1" t="n">
+        <v>3.5</v>
+      </c>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
@@ -7783,12 +8441,16 @@
       <c r="V218" s="2"/>
       <c r="W218" s="2"/>
     </row>
-    <row r="219" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B219" s="2"/>
-      <c r="C219" s="2"/>
+        <v>454</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C219" s="1" t="n">
+        <v>5.9</v>
+      </c>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
@@ -7810,12 +8472,16 @@
       <c r="V219" s="2"/>
       <c r="W219" s="2"/>
     </row>
-    <row r="220" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B220" s="2"/>
-      <c r="C220" s="2"/>
+        <v>456</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C220" s="1" t="n">
+        <v>0.6</v>
+      </c>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
@@ -7839,10 +8505,14 @@
     </row>
     <row r="221" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
+        <v>457</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C221" s="1" t="n">
+        <v>8.7</v>
+      </c>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
@@ -7864,12 +8534,16 @@
       <c r="V221" s="2"/>
       <c r="W221" s="2"/>
     </row>
-    <row r="222" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
+        <v>459</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C222" s="1" t="n">
+        <v>4.3</v>
+      </c>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
@@ -7891,12 +8565,16 @@
       <c r="V222" s="2"/>
       <c r="W222" s="2"/>
     </row>
-    <row r="223" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
+        <v>461</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C223" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
@@ -7918,12 +8596,16 @@
       <c r="V223" s="2"/>
       <c r="W223" s="2"/>
     </row>
-    <row r="224" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
+        <v>463</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C224" s="1" t="n">
+        <v>3.2</v>
+      </c>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
@@ -7945,12 +8627,16 @@
       <c r="V224" s="2"/>
       <c r="W224" s="2"/>
     </row>
-    <row r="225" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
+        <v>464</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C225" s="1" t="n">
+        <v>2.9</v>
+      </c>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
@@ -7972,12 +8658,16 @@
       <c r="V225" s="2"/>
       <c r="W225" s="2"/>
     </row>
-    <row r="226" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
+        <v>465</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C226" s="1" t="n">
+        <v>5.1</v>
+      </c>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
@@ -7999,12 +8689,16 @@
       <c r="V226" s="2"/>
       <c r="W226" s="2"/>
     </row>
-    <row r="227" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
+        <v>467</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C227" s="1" t="n">
+        <v>0.3</v>
+      </c>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
@@ -8026,12 +8720,16 @@
       <c r="V227" s="2"/>
       <c r="W227" s="2"/>
     </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B228" s="2"/>
-      <c r="C228" s="2"/>
+        <v>469</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C228" s="1" t="n">
+        <v>3.2</v>
+      </c>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
@@ -8053,12 +8751,16 @@
       <c r="V228" s="2"/>
       <c r="W228" s="2"/>
     </row>
-    <row r="229" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
+        <v>470</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C229" s="1" t="n">
+        <v>5.3</v>
+      </c>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
       <c r="F229" s="2"/>
@@ -8080,12 +8782,16 @@
       <c r="V229" s="2"/>
       <c r="W229" s="2"/>
     </row>
-    <row r="230" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="B230" s="2"/>
-      <c r="C230" s="2"/>
+        <v>472</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C230" s="1" t="n">
+        <v>1.1</v>
+      </c>
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
@@ -8107,12 +8813,16 @@
       <c r="V230" s="2"/>
       <c r="W230" s="2"/>
     </row>
-    <row r="231" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B231" s="2"/>
-      <c r="C231" s="2"/>
+        <v>473</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C231" s="1" t="n">
+        <v>3.7</v>
+      </c>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
@@ -8134,12 +8844,16 @@
       <c r="V231" s="2"/>
       <c r="W231" s="2"/>
     </row>
-    <row r="232" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B232" s="2"/>
-      <c r="C232" s="2"/>
+        <v>475</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C232" s="1" t="n">
+        <v>1.2</v>
+      </c>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
       <c r="F232" s="2"/>
@@ -8163,10 +8877,14 @@
     </row>
     <row r="233" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B233" s="2"/>
-      <c r="C233" s="2"/>
+        <v>477</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C233" s="1" t="n">
+        <v>2.7</v>
+      </c>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
       <c r="F233" s="2"/>
@@ -8188,12 +8906,16 @@
       <c r="V233" s="2"/>
       <c r="W233" s="2"/>
     </row>
-    <row r="234" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B234" s="2"/>
-      <c r="C234" s="2"/>
+        <v>479</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C234" s="1" t="n">
+        <v>3.2</v>
+      </c>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
@@ -8215,10 +8937,8 @@
       <c r="V234" s="2"/>
       <c r="W234" s="2"/>
     </row>
-    <row r="235" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="1" t="s">
-        <v>378</v>
-      </c>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="2"/>
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
@@ -27318,33 +28038,44 @@
       <c r="W998" s="2"/>
     </row>
     <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="2"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="2"/>
-      <c r="M999" s="2"/>
-      <c r="N999" s="2"/>
-      <c r="O999" s="2"/>
-      <c r="P999" s="2"/>
-      <c r="Q999" s="2"/>
-      <c r="R999" s="2"/>
-      <c r="S999" s="2"/>
-      <c r="T999" s="2"/>
-      <c r="U999" s="2"/>
-      <c r="V999" s="2"/>
-      <c r="W999" s="2"/>
+      <c r="A999" s="5"/>
+      <c r="B999" s="5"/>
+      <c r="C999" s="5"/>
+      <c r="D999" s="5"/>
+      <c r="E999" s="5"/>
+      <c r="F999" s="5"/>
+      <c r="G999" s="5"/>
+      <c r="H999" s="5"/>
+      <c r="I999" s="5"/>
+      <c r="J999" s="5"/>
+      <c r="K999" s="5"/>
+      <c r="L999" s="5"/>
+      <c r="M999" s="5"/>
+      <c r="N999" s="5"/>
+      <c r="O999" s="5"/>
+      <c r="P999" s="5"/>
+      <c r="Q999" s="5"/>
+      <c r="R999" s="5"/>
+      <c r="S999" s="5"/>
+      <c r="T999" s="5"/>
+      <c r="U999" s="5"/>
+      <c r="V999" s="5"/>
+      <c r="W999" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="jliew626@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://cccaustin.org/"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://austincitylife.org/"/>
+    <hyperlink ref="F3" r:id="rId3" display="INFO@AUSTINCITYLIFE.ORG"/>
+    <hyperlink ref="D4" r:id="rId4" display="https://www.ucc-austin.org/"/>
+    <hyperlink ref="F4" r:id="rId5" display="admin@ucc-austin.org"/>
+    <hyperlink ref="D5" r:id="rId6" display="https://cpcaustin.org/"/>
+    <hyperlink ref="F5" r:id="rId7" display="https://cpcaustin.org/contact/"/>
+    <hyperlink ref="D6" r:id="rId8" display="https://www.allsaints-austin.org/"/>
+    <hyperlink ref="D7" r:id="rId9" display="https://fumcaustin.org/"/>
+    <hyperlink ref="D8" r:id="rId10" display="https://austinstone.org/"/>
+    <hyperlink ref="F8" r:id="rId11" display="info@austinstone.org"/>
+    <hyperlink ref="D9" r:id="rId12" display="http://www.churchateast.com/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>